<commit_message>
ajout log commandes et fichiers
</commit_message>
<xml_diff>
--- a/data/Result_Course_Pronos_F1F_DEMO.xlsx
+++ b/data/Result_Course_Pronos_F1F_DEMO.xlsx
@@ -463,54 +463,54 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>la_bagguette</t>
+          <t>matt_karting</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ocon</t>
+          <t>z</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>HADJAR</t>
+          <t>z</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Gasly</t>
+          <t>z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Verstappen</t>
+          <t>z</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>matt_karting</t>
+          <t>palmer_jrr</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>vd</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>scv</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>scsv</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>vd</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Le grand nettoyage !!
</commit_message>
<xml_diff>
--- a/data/Result_Course_Pronos_F1F_DEMO.xlsx
+++ b/data/Result_Course_Pronos_F1F_DEMO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,22 +468,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>z</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>z</t>
+          <t>b</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>z</t>
+          <t>b</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>z</t>
+          <t>b</t>
         </is>
       </c>
     </row>
@@ -511,6 +511,33 @@
       <c r="E3" t="inlineStr">
         <is>
           <t>vd</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>la_bagguette</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Piastri</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Gasly</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Ocon</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Verstappen</t>
         </is>
       </c>
     </row>

</xml_diff>